<commit_message>
Update installer to use the interwebs
</commit_message>
<xml_diff>
--- a/Strafrunden/bin/Release/Test.xlsx
+++ b/Strafrunden/bin/Release/Test.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Strafrunden" sheetId="1" r:id="Rdc3b9349fe434e4b"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Strafrunden" sheetId="1" r:id="R01983b17b2524ce6"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -17,6 +17,31 @@
       <x:c t="str">
         <x:v>Strafrunden</x:v>
       </x:c>
+      <x:c t="str">
+        <x:v>Wurf-ID</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c t="n">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c t="n">
+        <x:v>432</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>2</x:v>
+      </x:c>
     </x:row>
     <x:row>
       <x:c t="n">
@@ -25,6 +50,31 @@
       <x:c t="n">
         <x:v>1</x:v>
       </x:c>
+      <x:c t="n">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c t="n">
+        <x:v>123</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c t="n">
+        <x:v>213</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c t="n">
+        <x:v>5</x:v>
+      </x:c>
     </x:row>
   </x:sheetData>
 </x:worksheet>

</xml_diff>